<commit_message>
comment 2 iranyu in progress
</commit_message>
<xml_diff>
--- a/WingtipToys/ReportTemplates/ReportTemplate.xlsx
+++ b/WingtipToys/ReportTemplates/ReportTemplate.xlsx
@@ -9,15 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="Kimutatás" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Munka1!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <pivotCaches>
+    <pivotCache cacheId="4" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Product name</t>
   </si>
@@ -39,6 +43,18 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>Sorcímkék</t>
+  </si>
+  <si>
+    <t>(üres)</t>
+  </si>
+  <si>
+    <t>Végösszeg</t>
+  </si>
+  <si>
+    <t>Mennyiség / Quantity</t>
   </si>
 </sst>
 </file>
@@ -75,8 +91,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -92,6 +113,1038 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="hu-HU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[ReportTemplate.xlsx]Kimutatás!Kimutatás1</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Kimutatás!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Összeg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Kimutatás!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(üres)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Kimutatás!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="226650960"/>
+        <c:axId val="273903400"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="226650960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="273903400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="273903400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226650960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Training" refreshedDate="42097.421049537035" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="1">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:D1048576" sheet="Munka1"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Product name" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Username" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Created" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Quantity" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
+  <r>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Kimutatás1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Értékek" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A1:B3" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Mennyiség / Quantity" fld="3" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,7 +1425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -404,4 +1457,44 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>